<commit_message>
fix(parallel for): fix paralelku
</commit_message>
<xml_diff>
--- a/OpenMP_Lab/result.xlsx
+++ b/OpenMP_Lab/result.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="(old)N=2k; cluster; -O3" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="(old)N=25k;laptop; -O2" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="(old)N=2k;laptop; -O2" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="(old)N=2k; laptop; -O3" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="N=25k; server; -O2" sheetId="5" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="10">
   <si>
     <t xml:space="preserve">Время</t>
   </si>
@@ -193,7 +194,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -247,6 +248,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -865,11 +874,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="44954932"/>
-        <c:axId val="75096667"/>
+        <c:axId val="98810486"/>
+        <c:axId val="5563406"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="44954932"/>
+        <c:axId val="98810486"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -901,12 +910,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75096667"/>
+        <c:crossAx val="5563406"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75096667"/>
+        <c:axId val="5563406"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -947,7 +956,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44954932"/>
+        <c:crossAx val="98810486"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1326,11 +1335,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="66853871"/>
-        <c:axId val="77957551"/>
+        <c:axId val="64126876"/>
+        <c:axId val="74293274"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="66853871"/>
+        <c:axId val="64126876"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1362,12 +1371,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77957551"/>
+        <c:crossAx val="74293274"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="77957551"/>
+        <c:axId val="74293274"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1408,7 +1417,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66853871"/>
+        <c:crossAx val="64126876"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1787,11 +1796,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="47042040"/>
-        <c:axId val="61085496"/>
+        <c:axId val="36316101"/>
+        <c:axId val="43320190"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="47042040"/>
+        <c:axId val="36316101"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1823,12 +1832,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61085496"/>
+        <c:crossAx val="43320190"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="61085496"/>
+        <c:axId val="43320190"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1869,7 +1878,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47042040"/>
+        <c:crossAx val="36316101"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2237,11 +2246,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="5481063"/>
-        <c:axId val="43842329"/>
+        <c:axId val="40242592"/>
+        <c:axId val="59329043"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="5481063"/>
+        <c:axId val="40242592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2273,12 +2282,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43842329"/>
+        <c:crossAx val="59329043"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="43842329"/>
+        <c:axId val="59329043"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2319,7 +2328,632 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5481063"/>
+        <c:crossAx val="40242592"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:ea typeface="DejaVu Sans"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0704309418646293"/>
+          <c:y val="0.0459696386572589"/>
+          <c:w val="0.750507341530381"/>
+          <c:h val="0.864870643574941"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="line"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="74389918"/>
+        <c:axId val="51133715"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="74389918"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="51133715"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="51133715"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="74389918"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:ea typeface="DejaVu Sans"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0702264196633975"/>
+          <c:y val="0.0461206896551724"/>
+          <c:w val="0.750454050127134"/>
+          <c:h val="0.864870689655172"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="line"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="15817218"/>
+        <c:axId val="62769155"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="15817218"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="62769155"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="62769155"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="15817218"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:ea typeface="DejaVu Sans"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="line"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="98997022"/>
+        <c:axId val="90551104"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="98997022"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="90551104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="90551104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="98997022"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2914,11 +3548,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="85202584"/>
-        <c:axId val="42696965"/>
+        <c:axId val="17282476"/>
+        <c:axId val="69085007"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85202584"/>
+        <c:axId val="17282476"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2950,12 +3584,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42696965"/>
+        <c:crossAx val="69085007"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="42696965"/>
+        <c:axId val="69085007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2996,7 +3630,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85202584"/>
+        <c:crossAx val="17282476"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3581,11 +4215,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="94896087"/>
-        <c:axId val="10105917"/>
+        <c:axId val="65496129"/>
+        <c:axId val="66491519"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="94896087"/>
+        <c:axId val="65496129"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3617,12 +4251,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10105917"/>
+        <c:crossAx val="66491519"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="10105917"/>
+        <c:axId val="66491519"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3663,7 +4297,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94896087"/>
+        <c:crossAx val="65496129"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4031,11 +4665,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="65655162"/>
-        <c:axId val="96932552"/>
+        <c:axId val="41471991"/>
+        <c:axId val="58655871"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="65655162"/>
+        <c:axId val="41471991"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4067,12 +4701,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96932552"/>
+        <c:crossAx val="58655871"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="96932552"/>
+        <c:axId val="58655871"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4113,7 +4747,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65655162"/>
+        <c:crossAx val="41471991"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4481,11 +5115,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="93669907"/>
-        <c:axId val="35772220"/>
+        <c:axId val="23443392"/>
+        <c:axId val="66364701"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="93669907"/>
+        <c:axId val="23443392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4517,12 +5151,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35772220"/>
+        <c:crossAx val="66364701"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="35772220"/>
+        <c:axId val="66364701"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4563,7 +5197,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93669907"/>
+        <c:crossAx val="23443392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4931,11 +5565,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="82119"/>
-        <c:axId val="32001825"/>
+        <c:axId val="28474040"/>
+        <c:axId val="32868096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="82119"/>
+        <c:axId val="28474040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4967,12 +5601,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32001825"/>
+        <c:crossAx val="32868096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="32001825"/>
+        <c:axId val="32868096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5013,7 +5647,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82119"/>
+        <c:crossAx val="28474040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5381,11 +6015,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="28128902"/>
-        <c:axId val="96457060"/>
+        <c:axId val="88056254"/>
+        <c:axId val="14610350"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="28128902"/>
+        <c:axId val="88056254"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5417,12 +6051,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96457060"/>
+        <c:crossAx val="14610350"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="96457060"/>
+        <c:axId val="14610350"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5463,7 +6097,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28128902"/>
+        <c:crossAx val="88056254"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5831,11 +6465,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="65343637"/>
-        <c:axId val="52586730"/>
+        <c:axId val="48121563"/>
+        <c:axId val="2017920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="65343637"/>
+        <c:axId val="48121563"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5867,12 +6501,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52586730"/>
+        <c:crossAx val="2017920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="52586730"/>
+        <c:axId val="2017920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5913,7 +6547,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65343637"/>
+        <c:crossAx val="48121563"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6281,11 +6915,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="86603775"/>
-        <c:axId val="18843260"/>
+        <c:axId val="86312860"/>
+        <c:axId val="54502703"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="86603775"/>
+        <c:axId val="86312860"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6317,12 +6951,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18843260"/>
+        <c:crossAx val="54502703"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="18843260"/>
+        <c:axId val="54502703"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6363,7 +6997,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86603775"/>
+        <c:crossAx val="86312860"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6832,6 +7466,101 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>111600</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>13320</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>477720</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>71280</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="111600" y="2289240"/>
+        <a:ext cx="3015360" cy="1683360"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>570240</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>44280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>183240</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>88560</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="14" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="3219480" y="2482560"/>
+        <a:ext cx="2972880" cy="1670040"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>8280</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>156240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>677160</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>77760</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="15" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="6017400" y="3895200"/>
+        <a:ext cx="3107160" cy="1872000"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
   <a:themeElements>
@@ -8249,8 +8978,8 @@
   </sheetPr>
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F33" activeCellId="0" sqref="F33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G29" activeCellId="0" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8569,4 +9298,438 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:Q26"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q2" activeCellId="0" sqref="Q2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.07"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="N1" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="O1" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="P1" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>232.864778</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>140.838924</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>98.714937</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>86.914779</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>74.887139</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>76.104112</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>73.396486</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>65.614899</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>60.244432</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>62.885586</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>65.750491</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>57.073289</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <v>65.096366</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <v>63.530195</v>
+      </c>
+      <c r="P2" s="0" t="n">
+        <v>60.45161</v>
+      </c>
+      <c r="Q2" s="0" t="n">
+        <v>57.551181</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>511.448068</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>352.437573</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>239.378091</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>166.067247</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>159.360383</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>132.19364</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>129.019905</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>117.32097</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>121.7052</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>113.50678</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>121.781834</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>109.85228</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>125.211012</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <v>132.125584</v>
+      </c>
+      <c r="P3" s="0" t="n">
+        <v>119.677091</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>120.171937</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>42.481455</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>22.85788</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>17.247888</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>14.922749</v>
+      </c>
+      <c r="F4" s="14"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F5" s="14"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <f aca="false">($B$2/B2)</f>
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <f aca="false">($B$2/C2)</f>
+        <v>1.65341207804172</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <f aca="false">($B$2/D2)</f>
+        <v>2.35896192690677</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <f aca="false">($B$2/E2)</f>
+        <v>2.67923108911086</v>
+      </c>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <f aca="false">($B$3/B3)</f>
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <f aca="false">($B$3/C3)</f>
+        <v>1.45117350470462</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <f aca="false">($B$3/D3)</f>
+        <v>2.13657008401826</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <f aca="false">($B$3/E3)</f>
+        <v>3.07976483767446</v>
+      </c>
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <f aca="false">($B$4/B4)</f>
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <f aca="false">($B$4/C4)</f>
+        <v>1.85850371950505</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <f aca="false">($B$4/D4)</f>
+        <v>2.46299459968664</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <f aca="false">($B$4/E4)</f>
+        <v>2.84675799345013</v>
+      </c>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F9" s="14"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <f aca="false">(B6/B1)*100</f>
+        <v>100</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <f aca="false">(C6/C1)*100</f>
+        <v>82.670603902086</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <f aca="false">(D6/D1)*100</f>
+        <v>78.6320642302255</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <f aca="false">(E6/E1)*100</f>
+        <v>66.9807772277716</v>
+      </c>
+      <c r="F10" s="14"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <f aca="false">(B7/B1)*100</f>
+        <v>100</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <f aca="false">(C7/C1)*100</f>
+        <v>72.558675235231</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <f aca="false">(D7/D1)*100</f>
+        <v>71.2190028006086</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <f aca="false">(E7/E1)*100</f>
+        <v>76.9941209418616</v>
+      </c>
+      <c r="F11" s="14"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <f aca="false">(B8/B1)*100</f>
+        <v>100</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <f aca="false">(C8/C1)*100</f>
+        <v>92.9251859752523</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <f aca="false">(D8/D1)*100</f>
+        <v>82.0998199895547</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <f aca="false">(E8/E1)*100</f>
+        <v>71.1689498362534</v>
+      </c>
+      <c r="F12" s="14"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F13" s="14"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="15"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7"/>
+      <c r="C16" s="7"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7"/>
+      <c r="C17" s="7"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7"/>
+      <c r="C18" s="7"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7"/>
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="7"/>
+      <c r="C20" s="7"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="7"/>
+      <c r="C21" s="7"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="7"/>
+      <c r="C22" s="7"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="7"/>
+      <c r="C23" s="7"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7"/>
+      <c r="C24" s="7"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7"/>
+      <c r="C25" s="7"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C26" s="7"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>